<commit_message>
Fixed tests and added Workbook command
</commit_message>
<xml_diff>
--- a/src/Tests/RegressionTests/Expected/Worksheets.xlsx
+++ b/src/Tests/RegressionTests/Expected/Worksheets.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <x:si>
     <x:t>January</x:t>
   </x:si>
@@ -53,6 +53,39 @@
     <x:t>December</x:t>
   </x:si>
   <x:si>
+    <x:t>Jan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Feb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jun</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jul</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aug</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sept</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oct</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nov</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dec</x:t>
+  </x:si>
+  <x:si>
     <x:t>січень</x:t>
   </x:si>
   <x:si>
@@ -87,6 +120,42 @@
   </x:si>
   <x:si>
     <x:t>грудень</x:t>
+  </x:si>
+  <x:si>
+    <x:t>січ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>лют</x:t>
+  </x:si>
+  <x:si>
+    <x:t>бер</x:t>
+  </x:si>
+  <x:si>
+    <x:t>кві</x:t>
+  </x:si>
+  <x:si>
+    <x:t>тра</x:t>
+  </x:si>
+  <x:si>
+    <x:t>чер</x:t>
+  </x:si>
+  <x:si>
+    <x:t>лип</x:t>
+  </x:si>
+  <x:si>
+    <x:t>сер</x:t>
+  </x:si>
+  <x:si>
+    <x:t>вер</x:t>
+  </x:si>
+  <x:si>
+    <x:t>жов</x:t>
+  </x:si>
+  <x:si>
+    <x:t>лис</x:t>
+  </x:si>
+  <x:si>
+    <x:t>гру</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -437,7 +506,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B12"/>
+  <x:dimension ref="A1:B24"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -537,6 +606,102 @@
       </x:c>
       <x:c r="B12" s="0" t="n">
         <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:2">
+      <x:c r="A14" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:2">
+      <x:c r="A15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:2">
+      <x:c r="A16" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:2">
+      <x:c r="A17" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:2">
+      <x:c r="A18" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:2">
+      <x:c r="A19" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:2">
+      <x:c r="A20" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:2">
+      <x:c r="A21" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:2">
+      <x:c r="A22" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:2">
+      <x:c r="A23" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:2">
+      <x:c r="A24" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="n">
+        <x:v>3</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -553,106 +718,205 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B12"/>
+  <x:dimension ref="A1:B24"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B1" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
+      <x:c r="C1" s="0">
+        <x:f>'English (United Kingdom)'!B1*2</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:2">
+    <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:2">
+    <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:2">
+    <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B5" s="0" t="n">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:2">
+    <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B6" s="0" t="n">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:2">
+    <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B7" s="0" t="n">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:2">
+    <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B8" s="0" t="n">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:2">
+    <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B9" s="0" t="n">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:2">
+    <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B10" s="0" t="n">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:2">
+    <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B11" s="0" t="n">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:2">
+    <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B12" s="0" t="n">
         <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:3">
+      <x:c r="A13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:3">
+      <x:c r="A14" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:3">
+      <x:c r="A15" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:3">
+      <x:c r="A16" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:3">
+      <x:c r="A17" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:3">
+      <x:c r="A18" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:3">
+      <x:c r="A19" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:3">
+      <x:c r="A20" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:3">
+      <x:c r="A21" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:3">
+      <x:c r="A22" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:3">
+      <x:c r="A23" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:3">
+      <x:c r="A24" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="n">
+        <x:v>3</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>